<commit_message>
Cambios archivos xlsx app y backend mejorias en el calculo de efectos
</commit_message>
<xml_diff>
--- a/data/Multiplicadores.xlsx
+++ b/data/Multiplicadores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juank\Documents\Practicas\CAMARA COMERCIO CGENA\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juank\turismo-religioso-analisis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DE812A-9C4C-4154-80C7-4BF40632C342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE0800D-832E-473B-9913-B8CA8E0E3108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4EB7F6F2-3930-46BE-8C56-7217EA629251}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
-    <t xml:space="preserve">Agrupaciones de actividades cuentas nacionales, según CIIU Rev. 4 A.C. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Agricultura y actividades de servicios conexas </t>
   </si>
   <si>
@@ -207,13 +204,16 @@
   </si>
   <si>
     <t>C_Sector</t>
+  </si>
+  <si>
+    <t>Sectores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,14 +223,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -273,9 +265,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -285,8 +274,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,7 +617,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,605 +626,605 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="C2">
         <v>1.1592652127250169</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1.1814298749063901</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1.207130112081974</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1.1376418538681019</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C6">
         <v>1.1771166268887072</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C8">
         <v>1.3454292406859834</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C9">
         <v>1.2628677537667445</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C10">
         <v>1.3469110230310568</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C11">
         <v>1.4270540057516194</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C13">
         <v>1.3726241279148559</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C14">
         <v>1.3533376527784373</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C17">
         <v>1.3276333704665326</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>17</v>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C18">
         <v>1.2056413801768626</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>18</v>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C19">
         <v>1.2481899434505872</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>19</v>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C20">
         <v>1.3216148772041083</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C21">
         <v>1.2962698622429372</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>21</v>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C22">
         <v>1.2962141780439309</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>22</v>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C23">
         <v>1.3117827973230209</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>23</v>
+      <c r="B24" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C24">
         <v>1.3733779306272493</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>24</v>
+      <c r="B25" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C25">
         <v>1.3278097314109294</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>25</v>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C26">
         <v>1.3754942341915786</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>26</v>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C27">
         <v>1.3580574123994449</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>27</v>
+      <c r="B28" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C28">
         <v>1.3999428406910568</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C29">
         <v>1.2562137894168242</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>29</v>
+      <c r="B30" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C30">
         <v>1.2180284386872215</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>30</v>
+      <c r="B31" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C31">
         <v>1.3289205421371564</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>31</v>
+      <c r="B32" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C32">
         <v>1.3154906169942473</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
+      <c r="B33" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C33">
         <v>1.1841962506714176</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>33</v>
+      <c r="B34" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C34">
         <v>1.7675805740026638</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>34</v>
+      <c r="B35" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C35">
         <v>1.4618099089497631</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>35</v>
+      <c r="B36" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C36">
         <v>1.4549338687575595</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>36</v>
+      <c r="B37" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C37">
         <v>1.4168132018615385</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>37</v>
+      <c r="B38" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C38">
         <v>1.4408623837343226</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>38</v>
+      <c r="B39" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C39">
         <v>1.3782755007468801</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>39</v>
+      <c r="B40" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C40">
         <v>1.2463240761263046</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>40</v>
+      <c r="B41" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C41">
         <v>1.35412970299567</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>41</v>
+      <c r="B42" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C42">
         <v>1.5081838781365249</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>42</v>
+      <c r="B43" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C43">
         <v>1.5174643923802262</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>43</v>
+      <c r="B44" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C44">
         <v>1.4365529881950738</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>44</v>
+      <c r="B45" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C45">
         <v>1.5436636579835905</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>45</v>
+      <c r="B46" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C46">
         <v>1.2657641256233143</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>46</v>
+      <c r="B47" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C47">
         <v>1.4160947266862947</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>47</v>
+      <c r="B48" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C48">
         <v>1.3218320693033283</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>48</v>
+      <c r="B49" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C49">
         <v>1.1049556733923445</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>49</v>
+      <c r="B50" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C50">
         <v>1.2612907842369021</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>50</v>
+      <c r="B51" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="C51">
         <v>1.4026987797275807</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>51</v>
+      <c r="B52" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C52">
         <v>1.2657962862850565</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>52</v>
+      <c r="B53" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C53">
         <v>1.5593192328713625</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>53</v>
+      <c r="B54" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C54">
         <v>1.2922017764671487</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
+      <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>54</v>
+      <c r="B55" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C55">
         <v>1</v>

</xml_diff>